<commit_message>
Edited until  Job 36:1
</commit_message>
<xml_diff>
--- a/Tools/work progress.xlsx
+++ b/Tools/work progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avi\GitHub\letteris\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4CC4B94-160D-4B1B-9B8C-16B5788D3668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D796537E-E245-411E-81C7-9F25D4B7C409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C244ACF4-AB16-42DE-8183-4B66D2E2F357}"/>
   </bookViews>
@@ -287,9 +287,6 @@
     <t>Book Number</t>
   </si>
   <si>
-    <t>Verses from beginning</t>
-  </si>
-  <si>
     <t>Verses in book</t>
   </si>
   <si>
@@ -300,13 +297,16 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>total verses in book from beginning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,6 +437,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -881,19 +887,20 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{A9FBBF1C-71F2-415F-81EE-920EAECC89A9}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="10" unboundColumnsRight="2">
+  <queryTableRefresh nextId="12" unboundColumnsRight="2">
     <queryTableFields count="6">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
-      <queryTableField id="5" name="Column5" tableColumnId="5"/>
+      <queryTableField id="11" dataBound="0" tableColumnId="3"/>
       <queryTableField id="7" dataBound="0" tableColumnId="7"/>
       <queryTableField id="6" name="Column6" tableColumnId="6"/>
       <queryTableField id="8" dataBound="0" tableColumnId="8"/>
       <queryTableField id="9" dataBound="0" tableColumnId="9"/>
     </queryTableFields>
-    <queryTableDeletedFields count="3">
+    <queryTableDeletedFields count="4">
       <deletedField name="Column2"/>
       <deletedField name="Column3"/>
       <deletedField name="Column4"/>
+      <deletedField name="Column5"/>
     </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
@@ -904,11 +911,11 @@
   <autoFilter ref="A1:F40" xr:uid="{3ABBE617-3032-4383-BD03-6F93CD160D46}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{AA516C31-175B-45AB-9CF7-F26D1794D44D}" uniqueName="1" name="Book Number" queryTableFieldId="1" dataDxfId="9" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5D8F6861-F3DD-4588-BAD1-9C98B8324DA5}" uniqueName="5" name="Verses from beginning" queryTableFieldId="5"/>
-    <tableColumn id="7" xr3:uid="{3D05ECBA-A37B-41CB-A300-26ED65F7D0A6}" uniqueName="7" name="Verses in book" queryTableFieldId="7" dataDxfId="7" totalsRowDxfId="3">
-      <calculatedColumnFormula>B2-C1</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{2642F5AC-5BE5-48DC-BD96-4F94451F41FC}" uniqueName="3" name="total verses in book from beginning" queryTableFieldId="11"/>
+    <tableColumn id="7" xr3:uid="{3D05ECBA-A37B-41CB-A300-26ED65F7D0A6}" uniqueName="7" name="Verses in book" queryTableFieldId="7" dataDxfId="8" totalsRowDxfId="3">
+      <calculatedColumnFormula>#REF!-C1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6D2EF4F8-2E7B-4DFE-96A8-C5E8779FACDA}" uniqueName="6" name="Book" queryTableFieldId="6" dataDxfId="8" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{6D2EF4F8-2E7B-4DFE-96A8-C5E8779FACDA}" uniqueName="6" name="Book" queryTableFieldId="6" dataDxfId="7" totalsRowDxfId="2"/>
     <tableColumn id="8" xr3:uid="{948872C3-C69C-49FA-940B-90AF18880A7B}" uniqueName="8" name="Verses done" totalsRowFunction="custom" queryTableFieldId="8" dataDxfId="6" totalsRowDxfId="1">
       <calculatedColumnFormula>IF(F2=1,C2,0)</calculatedColumnFormula>
       <totalsRowFormula>SUM(all[Verses done])</totalsRowFormula>
@@ -1221,13 +1228,13 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16.90625" customWidth="1"/>
   </cols>
@@ -1236,39 +1243,39 @@
       <c r="A1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D1" t="s">
         <v>78</v>
       </c>
       <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
         <v>82</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>15330</v>
+      <c r="B2" s="3">
+        <v>1533</v>
       </c>
       <c r="C2" s="3">
         <f>B2</f>
-        <v>15330</v>
+        <v>1533</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="1">
         <f t="shared" ref="E2:E40" si="0">IF(F2=1,C2,0)</f>
-        <v>15330</v>
+        <v>1533</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1278,19 +1285,19 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>27460</v>
+      <c r="B3" s="3">
+        <v>2746</v>
       </c>
       <c r="C3" s="3">
         <f>B3-B2</f>
-        <v>12130</v>
+        <v>1213</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" si="0"/>
-        <v>12130</v>
+        <v>1213</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -1300,19 +1307,19 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>36050</v>
+      <c r="B4" s="3">
+        <v>3605</v>
       </c>
       <c r="C4" s="3">
-        <f>B4-B3</f>
-        <v>8590</v>
+        <f t="shared" ref="C4:C40" si="1">B4-B3</f>
+        <v>859</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>8590</v>
+        <v>859</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
@@ -1322,19 +1329,19 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>48940</v>
+      <c r="B5" s="3">
+        <v>4894</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" ref="C5:C40" si="1">B5-B4</f>
-        <v>12890</v>
+        <f t="shared" si="1"/>
+        <v>1289</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>12890</v>
+        <v>1289</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -1344,19 +1351,19 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>58530</v>
+      <c r="B6" s="3">
+        <v>5853</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="1"/>
-        <v>9590</v>
+        <v>959</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>9590</v>
+        <v>959</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
@@ -1366,19 +1373,19 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>65110</v>
+      <c r="B7" s="3">
+        <v>6511</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="1"/>
-        <v>6580</v>
+        <v>658</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>6580</v>
+        <v>658</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -1388,19 +1395,19 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>71290</v>
+      <c r="B8" s="3">
+        <v>7129</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="1"/>
-        <v>6180</v>
+        <v>618</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>6180</v>
+        <v>618</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -1410,19 +1417,19 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>72140</v>
+      <c r="B9" s="3">
+        <v>7214</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="1"/>
-        <v>850</v>
+        <v>85</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>850</v>
+        <v>85</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
@@ -1432,19 +1439,19 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>80250</v>
+      <c r="B10" s="3">
+        <v>8025</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" si="1"/>
-        <v>8110</v>
+        <v>811</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>8110</v>
+        <v>811</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -1454,19 +1461,19 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>87200</v>
+      <c r="B11" s="3">
+        <v>8720</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" si="1"/>
-        <v>6950</v>
+        <v>695</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>6950</v>
+        <v>695</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
@@ -1476,19 +1483,19 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>95370</v>
+      <c r="B12" s="3">
+        <v>9537</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" si="1"/>
-        <v>8170</v>
+        <v>817</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>8170</v>
+        <v>817</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
@@ -1498,19 +1505,19 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>102560</v>
+      <c r="B13" s="3">
+        <v>10256</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" si="1"/>
-        <v>7190</v>
+        <v>719</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>50</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>7190</v>
+        <v>719</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -1520,19 +1527,19 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
-        <v>111990</v>
+      <c r="B14" s="3">
+        <v>11199</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="1"/>
-        <v>9430</v>
+        <v>943</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>9430</v>
+        <v>943</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -1542,19 +1549,19 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>120210</v>
+      <c r="B15" s="3">
+        <v>12021</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="1"/>
-        <v>8220</v>
+        <v>822</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>52</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>8220</v>
+        <v>822</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -1564,12 +1571,12 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>123010</v>
+      <c r="B16" s="3">
+        <v>12301</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="1"/>
-        <v>2800</v>
+        <v>280</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>53</v>
@@ -1584,12 +1591,12 @@
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>127060</v>
+      <c r="B17" s="3">
+        <v>12706</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="1"/>
-        <v>4050</v>
+        <v>405</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>54</v>
@@ -1604,12 +1611,12 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>128730</v>
+      <c r="B18" s="3">
+        <v>12873</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="1"/>
-        <v>1670</v>
+        <v>167</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>55</v>
@@ -1624,12 +1631,12 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
-        <v>139430</v>
+      <c r="B19" s="3">
+        <v>13943</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="1"/>
-        <v>10700</v>
+        <v>1070</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>56</v>
@@ -1639,26 +1646,26 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>164700</v>
+      <c r="B20" s="3">
+        <v>16470</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="1"/>
-        <v>25270</v>
+        <v>2527</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>25270</v>
+        <v>2527</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1668,19 +1675,19 @@
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>173850</v>
+      <c r="B21" s="3">
+        <v>17385</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" si="1"/>
-        <v>9150</v>
+        <v>915</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>9150</v>
+        <v>915</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -1690,19 +1697,19 @@
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>176070</v>
+      <c r="B22" s="3">
+        <v>17607</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="1"/>
-        <v>2220</v>
+        <v>222</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>2220</v>
+        <v>222</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1712,12 +1719,12 @@
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>177240</v>
+      <c r="B23" s="3">
+        <v>17724</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="1"/>
-        <v>1170</v>
+        <v>117</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>60</v>
@@ -1732,12 +1739,12 @@
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>190150</v>
+      <c r="B24" s="3">
+        <v>19015</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" si="1"/>
-        <v>12910</v>
+        <v>1291</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>61</v>
@@ -1752,12 +1759,12 @@
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>203790</v>
+      <c r="B25" s="3">
+        <v>20379</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="1"/>
-        <v>13640</v>
+        <v>1364</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>62</v>
@@ -1772,12 +1779,12 @@
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>205330</v>
+      <c r="B26" s="3">
+        <v>20533</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" si="1"/>
-        <v>1540</v>
+        <v>154</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>63</v>
@@ -1792,12 +1799,12 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>218060</v>
+      <c r="B27" s="3">
+        <v>21806</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="1"/>
-        <v>12730</v>
+        <v>1273</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>64</v>
@@ -1812,12 +1819,12 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
-        <v>221630</v>
+      <c r="B28" s="3">
+        <v>22163</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="1"/>
-        <v>3570</v>
+        <v>357</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>65</v>
@@ -1832,12 +1839,12 @@
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>223600</v>
+      <c r="B29" s="3">
+        <v>22360</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="1"/>
-        <v>1970</v>
+        <v>197</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>66</v>
@@ -1852,12 +1859,12 @@
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30">
-        <v>224330</v>
+      <c r="B30" s="3">
+        <v>22433</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="1"/>
-        <v>730</v>
+        <v>73</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>67</v>
@@ -1872,12 +1879,12 @@
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
-        <v>225790</v>
+      <c r="B31" s="3">
+        <v>22579</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="1"/>
-        <v>1460</v>
+        <v>146</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>68</v>
@@ -1892,12 +1899,12 @@
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
-        <v>226000</v>
+      <c r="B32" s="3">
+        <v>22600</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>21</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>69</v>
@@ -1912,12 +1919,12 @@
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>226480</v>
+      <c r="B33" s="3">
+        <v>22648</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>48</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>70</v>
@@ -1932,12 +1939,12 @@
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
-        <v>227530</v>
+      <c r="B34" s="3">
+        <v>22753</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" si="1"/>
-        <v>1050</v>
+        <v>105</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>71</v>
@@ -1952,12 +1959,12 @@
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
-        <v>228000</v>
+      <c r="B35" s="3">
+        <v>22800</v>
       </c>
       <c r="C35" s="3">
         <f t="shared" si="1"/>
-        <v>470</v>
+        <v>47</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>72</v>
@@ -1972,12 +1979,12 @@
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
-        <v>228560</v>
+      <c r="B36" s="3">
+        <v>22856</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" si="1"/>
-        <v>560</v>
+        <v>56</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>73</v>
@@ -1992,12 +1999,12 @@
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
-        <v>229090</v>
+      <c r="B37" s="3">
+        <v>22909</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" si="1"/>
-        <v>530</v>
+        <v>53</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>74</v>
@@ -2012,12 +2019,12 @@
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
-        <v>229470</v>
+      <c r="B38" s="3">
+        <v>22947</v>
       </c>
       <c r="C38" s="3">
         <f t="shared" si="1"/>
-        <v>380</v>
+        <v>38</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>75</v>
@@ -2032,12 +2039,12 @@
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
-        <v>231580</v>
+      <c r="B39" s="3">
+        <v>23158</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" si="1"/>
-        <v>2110</v>
+        <v>211</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>76</v>
@@ -2052,12 +2059,12 @@
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
-        <v>232130</v>
+      <c r="B40" s="3">
+        <v>23213</v>
       </c>
       <c r="C40" s="3">
         <f t="shared" si="1"/>
-        <v>550</v>
+        <v>55</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>77</v>
@@ -2074,7 +2081,7 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1">
         <f>SUM(all[Verses done])</f>
-        <v>156850</v>
+        <v>15685</v>
       </c>
       <c r="F41" s="1">
         <f>SUM(all[Book done])</f>
@@ -2092,6 +2099,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Edited until  Obadiah 1:1
</commit_message>
<xml_diff>
--- a/Tools/work progress.xlsx
+++ b/Tools/work progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avi\GitHub\letteris\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D796537E-E245-411E-81C7-9F25D4B7C409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D4BA22-BF80-4673-BDA6-35B4DC811B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C244ACF4-AB16-42DE-8183-4B66D2E2F357}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>01O</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>Book done</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>total verses in book from beginning</t>
@@ -1228,7 +1225,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1244,7 +1241,7 @@
         <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>80</v>
@@ -1643,10 +1640,10 @@
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>83</v>
+        <v>1070</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -2081,21 +2078,21 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1">
         <f>SUM(all[Verses done])</f>
-        <v>15685</v>
+        <v>16755</v>
       </c>
       <c r="F41" s="1">
         <f>SUM(all[Book done])</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E42" s="2">
         <f>all[[#Totals],[Verses done]]/B40</f>
-        <v>0.67569896178865296</v>
+        <v>0.72179382242708823</v>
       </c>
       <c r="F42" s="2">
         <f>all[[#Totals],[Book done]]/39</f>
-        <v>0.4358974358974359</v>
+        <v>0.46153846153846156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited until  Micah 2:8
</commit_message>
<xml_diff>
--- a/Tools/work progress.xlsx
+++ b/Tools/work progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avi\GitHub\letteris\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D4BA22-BF80-4673-BDA6-35B4DC811B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D570C74E-4879-4219-BDAB-BC3ECCA0B137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C244ACF4-AB16-42DE-8183-4B66D2E2F357}"/>
   </bookViews>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54B75CB-6760-4E00-8FBF-6DE3DD09999F}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1908,9 +1908,11 @@
       </c>
       <c r="E32" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
@@ -1928,9 +1930,11 @@
       </c>
       <c r="E33" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
@@ -2078,21 +2082,21 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1">
         <f>SUM(all[Verses done])</f>
-        <v>16755</v>
+        <v>16824</v>
       </c>
       <c r="F41" s="1">
         <f>SUM(all[Book done])</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E42" s="2">
         <f>all[[#Totals],[Verses done]]/B40</f>
-        <v>0.72179382242708823</v>
+        <v>0.72476629474863219</v>
       </c>
       <c r="F42" s="2">
         <f>all[[#Totals],[Book done]]/39</f>
-        <v>0.46153846153846156</v>
+        <v>0.51282051282051277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited until  Ezekiel 1:5
</commit_message>
<xml_diff>
--- a/Tools/work progress.xlsx
+++ b/Tools/work progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avi\GitHub\letteris\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D18FC9-A41D-42AA-97D9-073BE0A5F2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71ADD2E-5EFE-45DD-8415-BE73A5AFDA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C244ACF4-AB16-42DE-8183-4B66D2E2F357}"/>
   </bookViews>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54B75CB-6760-4E00-8FBF-6DE3DD09999F}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F42" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1728,9 +1728,11 @@
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>117</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
@@ -1770,9 +1772,11 @@
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>1364</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
@@ -1790,9 +1794,11 @@
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
@@ -2096,21 +2102,21 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1">
         <f>SUM(all[Verses done])</f>
-        <v>18739</v>
+        <v>20374</v>
       </c>
       <c r="F41" s="1">
         <f>SUM(all[Book done])</f>
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E42" s="2">
         <f>all[[#Totals],[Verses done]]/B40</f>
-        <v>0.80726317149872917</v>
+        <v>0.87769784172661869</v>
       </c>
       <c r="F42" s="2">
         <f>all[[#Totals],[Book done]]/39</f>
-        <v>0.69230769230769229</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited until  Nehemiah 2:10
</commit_message>
<xml_diff>
--- a/Tools/work progress.xlsx
+++ b/Tools/work progress.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avi\GitHub\letteris\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71ADD2E-5EFE-45DD-8415-BE73A5AFDA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9570B86F-F48B-42E0-89E9-F77AE295C0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C244ACF4-AB16-42DE-8183-4B66D2E2F357}"/>
   </bookViews>
@@ -1225,7 +1225,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F42" sqref="A1:F42"/>
+      <selection activeCell="E40" sqref="A2:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1580,9 +1580,11 @@
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="1"/>
+        <v>280</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
@@ -1620,9 +1622,11 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
@@ -1816,9 +1820,11 @@
       </c>
       <c r="E27" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>1273</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
@@ -1836,9 +1842,11 @@
       </c>
       <c r="E28" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="1"/>
+        <v>357</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
@@ -2032,9 +2040,11 @@
       </c>
       <c r="E37" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
@@ -2052,9 +2062,11 @@
       </c>
       <c r="E38" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
@@ -2072,9 +2084,11 @@
       </c>
       <c r="E39" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>211</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
@@ -2092,9 +2106,11 @@
       </c>
       <c r="E40" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
@@ -2102,21 +2118,21 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1">
         <f>SUM(all[Verses done])</f>
-        <v>20374</v>
+        <v>22808</v>
       </c>
       <c r="F41" s="1">
         <f>SUM(all[Book done])</f>
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E42" s="2">
         <f>all[[#Totals],[Verses done]]/B40</f>
-        <v>0.87769784172661869</v>
+        <v>0.98255287985180717</v>
       </c>
       <c r="F42" s="2">
         <f>all[[#Totals],[Book done]]/39</f>
-        <v>0.76923076923076927</v>
+        <v>0.97435897435897434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>